<commit_message>
updated 24th september monday 2018
</commit_message>
<xml_diff>
--- a/neelma_september_timesheet.xlsx
+++ b/neelma_september_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t xml:space="preserve">employee name:</t>
   </si>
@@ -185,39 +185,60 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">1.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">saturday</t>
   </si>
   <si>
     <t xml:space="preserve">OFF</t>
   </si>
   <si>
+    <t xml:space="preserve">2.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">sunday</t>
   </si>
   <si>
+    <t xml:space="preserve">3.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">monday</t>
   </si>
   <si>
     <t xml:space="preserve">read python basics</t>
   </si>
   <si>
+    <t xml:space="preserve">4.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">tuesday</t>
   </si>
   <si>
     <t xml:space="preserve">read python loops and functions</t>
   </si>
   <si>
+    <t xml:space="preserve">5.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">wednesday</t>
   </si>
   <si>
     <t xml:space="preserve">read python file handling</t>
   </si>
   <si>
+    <t xml:space="preserve">6.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">thursday</t>
   </si>
   <si>
     <t xml:space="preserve">arrays in python</t>
   </si>
   <si>
+    <t xml:space="preserve">7.9.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">friday</t>
   </si>
   <si>
@@ -293,6 +314,9 @@
     <t xml:space="preserve">19.9.18</t>
   </si>
   <si>
+    <t xml:space="preserve">learnt about odoo </t>
+  </si>
+  <si>
     <t xml:space="preserve">20.9.18</t>
   </si>
   <si>
@@ -309,6 +333,9 @@
   </si>
   <si>
     <t xml:space="preserve">24.9.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried some basic commmands of linux CLI and started php</t>
   </si>
   <si>
     <t xml:space="preserve">25.9.18</t>
@@ -811,21 +838,21 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="44.2755102040816"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -979,7 +1006,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="13" t="n">
         <f aca="false">I47</f>
-        <v>0.666666666666666</v>
+        <v>0.916666666666666</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
@@ -996,7 +1023,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="13" t="n">
         <f aca="false">I57</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
@@ -1013,7 +1040,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="n">
         <f aca="false">SUM(D9:E12)</f>
-        <v>4.00000000000001</v>
+        <v>4.58333333333334</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
@@ -1114,11 +1141,11 @@
     </row>
     <row r="20" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
-      <c r="B20" s="24" t="n">
-        <v>43109</v>
+      <c r="B20" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
@@ -1130,16 +1157,16 @@
         <v>0</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="19"/>
-      <c r="B21" s="24" t="n">
-        <v>43140</v>
+      <c r="B21" s="24" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
@@ -1151,16 +1178,16 @@
         <v>0</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
-      <c r="B22" s="24" t="n">
-        <v>43168</v>
+      <c r="B22" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
@@ -1176,16 +1203,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="19"/>
-      <c r="B23" s="24" t="n">
-        <v>43199</v>
+      <c r="B23" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
@@ -1201,16 +1228,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
-      <c r="B24" s="24" t="n">
-        <v>43229</v>
+      <c r="B24" s="24" t="s">
+        <v>29</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
@@ -1226,16 +1253,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J24" s="32" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
-      <c r="B25" s="24" t="n">
-        <v>43260</v>
+      <c r="B25" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
@@ -1251,16 +1278,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
-      <c r="B26" s="24" t="n">
-        <v>43290</v>
+      <c r="B26" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
@@ -1276,7 +1303,7 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J26" s="32" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1288,7 +1315,7 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="35" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I27" s="36" t="n">
         <f aca="false">SUM(I20:I26)</f>
@@ -1333,16 +1360,16 @@
         <v>16</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="19"/>
       <c r="B30" s="24" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="27"/>
@@ -1354,16 +1381,16 @@
         <v>0</v>
       </c>
       <c r="J30" s="31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="19"/>
       <c r="B31" s="24" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="27"/>
@@ -1375,16 +1402,16 @@
         <v>0</v>
       </c>
       <c r="J31" s="31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="19"/>
       <c r="B32" s="24" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
@@ -1400,16 +1427,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J32" s="31" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="19"/>
       <c r="B33" s="24" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="27"/>
@@ -1425,16 +1452,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="19"/>
       <c r="B34" s="24" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="27"/>
@@ -1450,16 +1477,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="19"/>
       <c r="B35" s="24" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
@@ -1475,16 +1502,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="19"/>
       <c r="B36" s="24" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="27"/>
@@ -1500,7 +1527,7 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J36" s="32" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1512,7 +1539,7 @@
       <c r="F37" s="34"/>
       <c r="G37" s="34"/>
       <c r="H37" s="35" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I37" s="36" t="n">
         <f aca="false">SUM(I30:I36)</f>
@@ -1557,16 +1584,16 @@
         <v>16</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="19"/>
       <c r="B40" s="24" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D40" s="26"/>
       <c r="E40" s="27"/>
@@ -1578,16 +1605,16 @@
         <v>0</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="19"/>
       <c r="B41" s="24" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D41" s="26"/>
       <c r="E41" s="27"/>
@@ -1599,16 +1626,16 @@
         <v>0</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="19"/>
       <c r="B42" s="24" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="27"/>
@@ -1624,16 +1651,16 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J42" s="32" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="19"/>
       <c r="B43" s="24" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="27"/>
@@ -1649,35 +1676,41 @@
         <v>0.333333333333333</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="19"/>
       <c r="B44" s="24" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" s="26"/>
       <c r="E44" s="27"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="26"/>
+      <c r="G44" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H44" s="26" t="n">
+        <v>0.666666666666667</v>
+      </c>
       <c r="I44" s="30" t="n">
         <f aca="false">(E44-D44)+(H44-G44)</f>
-        <v>0</v>
-      </c>
-      <c r="J44" s="32"/>
+        <v>0.25</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="19"/>
       <c r="B45" s="24" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D45" s="26"/>
       <c r="E45" s="27"/>
@@ -1688,15 +1721,17 @@
         <f aca="false">(E45-D45)+(H45-G45)</f>
         <v>0</v>
       </c>
-      <c r="J45" s="32"/>
+      <c r="J45" s="32" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="19"/>
       <c r="B46" s="24" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D46" s="26"/>
       <c r="E46" s="27"/>
@@ -1707,7 +1742,9 @@
         <f aca="false">(E46-D46)+(H46-G46)</f>
         <v>0</v>
       </c>
-      <c r="J46" s="32"/>
+      <c r="J46" s="32" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="19"/>
@@ -1718,11 +1755,11 @@
       <c r="F47" s="34"/>
       <c r="G47" s="34"/>
       <c r="H47" s="35" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="I47" s="36" t="n">
         <f aca="false">SUM(I40:I46)</f>
-        <v>0.666666666666666</v>
+        <v>0.916666666666666</v>
       </c>
       <c r="J47" s="19"/>
     </row>
@@ -1763,16 +1800,16 @@
         <v>16</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="19"/>
       <c r="B50" s="24" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D50" s="26"/>
       <c r="E50" s="27"/>
@@ -1783,15 +1820,17 @@
         <f aca="false">(E50-D50)+(H50-G50)</f>
         <v>0</v>
       </c>
-      <c r="J50" s="31"/>
+      <c r="J50" s="31" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="19"/>
       <c r="B51" s="37" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D51" s="26"/>
       <c r="E51" s="27"/>
@@ -1802,34 +1841,42 @@
         <f aca="false">(E51-D51)+(H51-G51)</f>
         <v>0</v>
       </c>
-      <c r="J51" s="31"/>
+      <c r="J51" s="31" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="19"/>
       <c r="B52" s="37" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="27"/>
       <c r="F52" s="28"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="26"/>
+      <c r="G52" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H52" s="26" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I52" s="30" t="n">
         <f aca="false">(E52-D52)+(H52-G52)</f>
-        <v>0</v>
-      </c>
-      <c r="J52" s="32"/>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J52" s="32" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="19"/>
       <c r="B53" s="37" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D53" s="26"/>
       <c r="E53" s="27"/>
@@ -1845,10 +1892,10 @@
     <row r="54" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="19"/>
       <c r="B54" s="37" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="27"/>
@@ -1864,10 +1911,10 @@
     <row r="55" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="19"/>
       <c r="B55" s="37" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="27"/>
@@ -1883,10 +1930,10 @@
     <row r="56" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="19"/>
       <c r="B56" s="37" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D56" s="26"/>
       <c r="E56" s="27"/>
@@ -1908,11 +1955,11 @@
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
       <c r="H57" s="35" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="I57" s="36" t="n">
         <f aca="false">SUM(I50:I56)</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J57" s="19"/>
     </row>
@@ -1955,7 +2002,7 @@
     <row r="61" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="19"/>
       <c r="B61" s="42" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="43"/>
@@ -1969,7 +2016,7 @@
     <row r="62" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="19"/>
       <c r="B62" s="42" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="43"/>

</xml_diff>

<commit_message>
updated 26th september 2018 wednesday
</commit_message>
<xml_diff>
--- a/neelma_september_timesheet.xlsx
+++ b/neelma_september_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
   <si>
     <t xml:space="preserve">employee name:</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t xml:space="preserve">26.9.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watched tutorials of using SQL with oracle SQL developer and loops and function in php</t>
   </si>
   <si>
     <t xml:space="preserve">27.9.18</t>
@@ -838,22 +841,23 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1023,7 +1027,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="13" t="n">
         <f aca="false">I57</f>
-        <v>0.333333333333333</v>
+        <v>0.666666666666666</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
@@ -1040,7 +1044,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="n">
         <f aca="false">SUM(D9:E12)</f>
-        <v>4.58333333333334</v>
+        <v>4.91666666666667</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
@@ -1887,7 +1891,9 @@
         <f aca="false">(E53-D53)+(H53-G53)</f>
         <v>0</v>
       </c>
-      <c r="J53" s="32"/>
+      <c r="J53" s="32" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="19"/>
@@ -1900,18 +1906,24 @@
       <c r="D54" s="26"/>
       <c r="E54" s="27"/>
       <c r="F54" s="28"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="26"/>
+      <c r="G54" s="29" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="H54" s="26" t="n">
+        <v>0.770833333333333</v>
+      </c>
       <c r="I54" s="30" t="n">
         <f aca="false">(E54-D54)+(H54-G54)</f>
-        <v>0</v>
-      </c>
-      <c r="J54" s="32"/>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J54" s="32" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="19"/>
       <c r="B55" s="37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>33</v>
@@ -1930,7 +1942,7 @@
     <row r="56" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="19"/>
       <c r="B56" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>36</v>
@@ -1955,11 +1967,11 @@
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
       <c r="H57" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I57" s="36" t="n">
         <f aca="false">SUM(I50:I56)</f>
-        <v>0.333333333333333</v>
+        <v>0.666666666666666</v>
       </c>
       <c r="J57" s="19"/>
     </row>
@@ -2002,7 +2014,7 @@
     <row r="61" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="19"/>
       <c r="B61" s="42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="43"/>
@@ -2016,7 +2028,7 @@
     <row r="62" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="19"/>
       <c r="B62" s="42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="43"/>

</xml_diff>

<commit_message>
updated 27th september 2018 thursday
</commit_message>
<xml_diff>
--- a/neelma_september_timesheet.xlsx
+++ b/neelma_september_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
   <si>
     <t xml:space="preserve">employee name:</t>
   </si>
@@ -344,10 +344,13 @@
     <t xml:space="preserve">26.9.18</t>
   </si>
   <si>
-    <t xml:space="preserve">watched tutorials of using SQL with oracle SQL developer and loops and function in php</t>
+    <t xml:space="preserve">watched tutorials of using SQL with oracle SQL developer and loops and functions in php</t>
   </si>
   <si>
     <t xml:space="preserve">27.9.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">php arrays sorting, file handling, form handling </t>
   </si>
   <si>
     <t xml:space="preserve">28.9.18</t>
@@ -841,22 +844,22 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J56" activeCellId="0" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.7142857142857"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
@@ -1027,7 +1030,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="13" t="n">
         <f aca="false">I57</f>
-        <v>0.666666666666666</v>
+        <v>1.01388888888889</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
@@ -1044,7 +1047,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="n">
         <f aca="false">SUM(D9:E12)</f>
-        <v>4.91666666666667</v>
+        <v>5.26388888888889</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
@@ -1931,18 +1934,24 @@
       <c r="D55" s="26"/>
       <c r="E55" s="27"/>
       <c r="F55" s="28"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="26"/>
+      <c r="G55" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H55" s="26" t="n">
+        <v>0.763888888888889</v>
+      </c>
       <c r="I55" s="30" t="n">
         <f aca="false">(E55-D55)+(H55-G55)</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="32"/>
+        <v>0.347222222222222</v>
+      </c>
+      <c r="J55" s="32" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="19"/>
       <c r="B56" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>36</v>
@@ -1967,11 +1976,11 @@
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
       <c r="H57" s="35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I57" s="36" t="n">
         <f aca="false">SUM(I50:I56)</f>
-        <v>0.666666666666666</v>
+        <v>1.01388888888889</v>
       </c>
       <c r="J57" s="19"/>
     </row>
@@ -2014,7 +2023,7 @@
     <row r="61" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="19"/>
       <c r="B61" s="42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="43"/>
@@ -2028,7 +2037,7 @@
     <row r="62" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="19"/>
       <c r="B62" s="42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="43"/>

</xml_diff>

<commit_message>
updated 28th september 2018 friday
</commit_message>
<xml_diff>
--- a/neelma_september_timesheet.xlsx
+++ b/neelma_september_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t xml:space="preserve">employee name:</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t xml:space="preserve">28.9.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHP with SQL </t>
   </si>
   <si>
     <t xml:space="preserve">Total Hours (4th Week)</t>
@@ -844,23 +847,23 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J56" activeCellId="0" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1030,7 +1033,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="13" t="n">
         <f aca="false">I57</f>
-        <v>1.01388888888889</v>
+        <v>1.36805555555556</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
@@ -1047,7 +1050,7 @@
       <c r="C13" s="15"/>
       <c r="D13" s="16" t="n">
         <f aca="false">SUM(D9:E12)</f>
-        <v>5.26388888888889</v>
+        <v>5.61805555555556</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
@@ -1959,13 +1962,19 @@
       <c r="D56" s="26"/>
       <c r="E56" s="27"/>
       <c r="F56" s="33"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="26"/>
+      <c r="G56" s="29" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="H56" s="26" t="n">
+        <v>0.770833333333333</v>
+      </c>
       <c r="I56" s="30" t="n">
         <f aca="false">(E56-D56)+(H56-G56)</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="32"/>
+        <v>0.354166666666667</v>
+      </c>
+      <c r="J56" s="32" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="19"/>
@@ -1976,11 +1985,11 @@
       <c r="F57" s="34"/>
       <c r="G57" s="34"/>
       <c r="H57" s="35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I57" s="36" t="n">
         <f aca="false">SUM(I50:I56)</f>
-        <v>1.01388888888889</v>
+        <v>1.36805555555556</v>
       </c>
       <c r="J57" s="19"/>
     </row>
@@ -2023,7 +2032,7 @@
     <row r="61" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="19"/>
       <c r="B61" s="42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="43"/>
@@ -2037,7 +2046,7 @@
     <row r="62" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="19"/>
       <c r="B62" s="42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="43"/>

</xml_diff>